<commit_message>
Admin Page bug fix
</commit_message>
<xml_diff>
--- a/admin/holidays/uploads/holiday.xlsx
+++ b/admin/holidays/uploads/holiday.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRAVEEN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A237BA38-63D4-44EF-96AC-BABE9EC923CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19B4AA0-EBAE-4A34-8121-C8C14E6740B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11640" yWindow="348" windowWidth="11400" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,7 +364,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,23 +390,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>45305</v>
+        <v>45317</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>45317</v>
+        <v>45297</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>45297</v>
+        <v>45304</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -414,7 +414,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>45304</v>
+        <v>45311</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>45311</v>
+        <v>45318</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -430,10 +430,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>45318</v>
+        <v>45306</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>